<commit_message>
Poke at stuff to form the final version.
</commit_message>
<xml_diff>
--- a/notes.xlsx
+++ b/notes.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tom/beeb/code/256_bytes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DD8C255-7139-8345-AEFA-F86F508E3D07}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BCED68D-9E24-6644-8FD2-BDD31FBDC582}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28800" yWindow="0" windowWidth="28800" windowHeight="34120" activeTab="1" xr2:uid="{E5D46CD9-8C28-8B42-BB43-C26FE315D941}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" activeTab="1" xr2:uid="{E5D46CD9-8C28-8B42-BB43-C26FE315D941}"/>
   </bookViews>
   <sheets>
     <sheet name="notes" sheetId="1" r:id="rId1"/>
     <sheet name="beeb SN frequencies" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="32">
   <si>
     <t>scale</t>
   </si>
@@ -98,6 +98,30 @@
   </si>
   <si>
     <t>B3</t>
+  </si>
+  <si>
+    <t>C4</t>
+  </si>
+  <si>
+    <t>G4</t>
+  </si>
+  <si>
+    <t>E4</t>
+  </si>
+  <si>
+    <t>F4</t>
+  </si>
+  <si>
+    <t>A4</t>
+  </si>
+  <si>
+    <t>D4</t>
+  </si>
+  <si>
+    <t>B4</t>
+  </si>
+  <si>
+    <t>F#4</t>
   </si>
 </sst>
 </file>
@@ -463,7 +487,7 @@
   <dimension ref="A1:B15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:B15"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -602,8 +626,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A801D82F-BDE4-F144-A9CA-676F32249B65}">
   <dimension ref="A1:O1025"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O33" sqref="O33"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="G27" sqref="G27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1458,6 +1482,9 @@
         <f t="shared" si="6"/>
         <v>488.28125</v>
       </c>
+      <c r="O18" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.2">
       <c r="D19">
@@ -1542,6 +1569,9 @@
         <f t="shared" si="6"/>
         <v>434.02777777777777</v>
       </c>
+      <c r="O20" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.2">
       <c r="D21">
@@ -1629,6 +1659,9 @@
         <f t="shared" si="6"/>
         <v>390.625</v>
       </c>
+      <c r="O22" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.2">
       <c r="D23">
@@ -1671,6 +1704,9 @@
         <f t="shared" si="6"/>
         <v>372.02380952380952</v>
       </c>
+      <c r="O23" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.2">
       <c r="D24">
@@ -1713,6 +1749,9 @@
         <f t="shared" si="6"/>
         <v>355.11363636363637</v>
       </c>
+      <c r="O24" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.2">
       <c r="D25">
@@ -1800,6 +1839,9 @@
         <f t="shared" si="6"/>
         <v>325.52083333333331</v>
       </c>
+      <c r="O26" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.2">
       <c r="D27">
@@ -1926,6 +1968,9 @@
         <f t="shared" si="6"/>
         <v>289.35185185185185</v>
       </c>
+      <c r="O29" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.2">
       <c r="D30">
@@ -2052,6 +2097,9 @@
         <f t="shared" si="6"/>
         <v>260.41666666666669</v>
       </c>
+      <c r="O32" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="33" spans="4:15" x14ac:dyDescent="0.2">
       <c r="D33">

</xml_diff>